<commit_message>
Fixed notes in TrainingComparison.xlsx
</commit_message>
<xml_diff>
--- a/tensorflow/columns_experiment_win_middle/TrainingComparison.xlsx
+++ b/tensorflow/columns_experiment_win_middle/TrainingComparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Gen Nishida\Documents\GitHub\FacadeAnnotationTool\tensorflow\columns_experiment_win_middle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464B73F3-C089-4D1C-AC64-54086C622800}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE79238-F604-49AD-893A-BEA7324BF8E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="3105" windowWidth="22905" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="615" yWindow="3045" windowWidth="22905" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,20 +62,20 @@
     <t>x20</t>
   </si>
   <si>
-    <t>Adjust y according to the random crop
+    <t>Shift [-4, 4]
+rotate [-0.5, 0.5]</t>
+  </si>
+  <si>
+    <t>Shift [-4, 4]
+rotate [-0.1, 0.1]</t>
+  </si>
+  <si>
+    <t>Adjust param according to the random crop
 Grayscale
 Use border between windows</t>
   </si>
   <si>
-    <t>Shift [-4, 4]
-rotate [-0.5, 0.5]</t>
-  </si>
-  <si>
-    <t>Shift [-4, 4]
-rotate [-0.1, 0.1]</t>
-  </si>
-  <si>
-    <t>Adjust y according to the random crop
+    <t>Adjust param according to the random crop
 Grayscale
 Use border between windows
 Crop sky and shop</t>
@@ -445,7 +445,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -503,10 +503,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>10</v>
@@ -573,7 +573,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Added columns_experiment 9 and 10
</commit_message>
<xml_diff>
--- a/tensorflow/columns_experiment_win_middle/TrainingComparison.xlsx
+++ b/tensorflow/columns_experiment_win_middle/TrainingComparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\taiga\Documents\GitHub\FacadeAnnotationTool\tensorflow\columns_experiment_win_middle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Gen Nishida\Documents\GitHub\FacadeAnnotationTool\tensorflow\columns_experiment_win_middle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E2B928-F479-4212-B61C-F80BB4C40CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD08DAE-ABB7-4E53-BC65-9F22890B6B2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="1155" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4230" yWindow="1470" windowWidth="23730" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>Model</t>
   </si>
@@ -117,6 +117,14 @@
 + Dropout
 + Dense(512, relu, regularizer)
 + Dropout</t>
+  </si>
+  <si>
+    <t>Shift [-4, 4] (mode='edge')
+rotate [-0.5, 0.5]</t>
+  </si>
+  <si>
+    <t>Shift [-4, 4] (mode='edge')
+rotate [-0.5, 0.5] (mode='nearest')</t>
   </si>
 </sst>
 </file>
@@ -516,17 +524,17 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="6" width="8.42578125" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" customWidth="1"/>
@@ -849,35 +857,75 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="14">
+        <v>1E-4</v>
+      </c>
+      <c r="G10" s="14">
+        <v>60</v>
+      </c>
+      <c r="H10" s="15">
+        <v>1.01E-2</v>
+      </c>
+      <c r="I10" s="12">
+        <v>1.7908E-4</v>
+      </c>
+      <c r="J10" s="16">
+        <v>2.3400000000000001E-2</v>
+      </c>
+      <c r="K10" s="12">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="7"/>
+      <c r="B11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="14">
+        <v>1E-4</v>
+      </c>
+      <c r="G11" s="14">
+        <v>60</v>
+      </c>
+      <c r="H11" s="10">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="I11" s="7">
+        <v>1.6636999999999999E-4</v>
+      </c>
+      <c r="J11" s="11">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="K11" s="7">
+        <v>7.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">

</xml_diff>